<commit_message>
Nice one My Self
</commit_message>
<xml_diff>
--- a/DataFrame of T.kholed/newdata.xlsx
+++ b/DataFrame of T.kholed/newdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TUF GAMING\Documents\GitHub\data-science-with-python-2022\DataFrame of T.kholed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5429A34C-00FD-4C1C-BC6E-AB1CAE68498F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E9F72F-B260-40DB-BE7C-C56CF684E9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B7D808BE-9E23-4771-9E56-D23ADCE2ADA6}"/>
   </bookViews>
@@ -34,16 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="46">
-  <si>
-    <t>ปีการศึกษา</t>
-  </si>
-  <si>
-    <t>ภาคการศึกษา</t>
-  </si>
-  <si>
-    <t>รหัสวิชา</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="43">
   <si>
     <t>GE219-501</t>
   </si>
@@ -117,21 +108,6 @@
     <t>GE2300-321</t>
   </si>
   <si>
-    <t>DS2303-316</t>
-  </si>
-  <si>
-    <t>DS2303-317</t>
-  </si>
-  <si>
-    <t>DS2303-323</t>
-  </si>
-  <si>
-    <t>IT2301-214</t>
-  </si>
-  <si>
-    <t>IT2301-229</t>
-  </si>
-  <si>
     <t>IT231-104  ( Close )</t>
   </si>
   <si>
@@ -147,31 +123,46 @@
     <t>IT2301-452  ( Close )</t>
   </si>
   <si>
-    <t>กลุ่ม</t>
+    <t>Term Group</t>
   </si>
   <si>
-    <t>จำนวนรับ</t>
+    <t>Year Group</t>
   </si>
   <si>
-    <t>ลงแล้ว</t>
+    <t>People</t>
   </si>
   <si>
-    <t>คอร์ส</t>
+    <t>Hours</t>
   </si>
   <si>
-    <t>ชั่วโมง</t>
+    <t>Course</t>
   </si>
   <si>
-    <t>คน</t>
+    <t>Limit</t>
   </si>
   <si>
-    <t>รวมลง</t>
+    <t>Group</t>
   </si>
   <si>
-    <t>รวมกลุ่มรายปี</t>
+    <t>Subject No.</t>
   </si>
   <si>
-    <t>รวมกลุ่มรายเทอม</t>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Registered</t>
+  </si>
+  <si>
+    <t>All student</t>
+  </si>
+  <si>
+    <t>S_Year</t>
+  </si>
+  <si>
+    <t>S_AS</t>
   </si>
 </sst>
 </file>
@@ -538,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC4E633-08E2-4543-9753-AE87DF5DD1FC}">
-  <dimension ref="A1:L132"/>
+  <dimension ref="A1:N132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="D134" sqref="D134"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,45 +542,51 @@
     <col min="11" max="11" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>39</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>2554</v>
       </c>
@@ -597,7 +594,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -626,8 +623,14 @@
       <c r="L2" s="1">
         <v>144</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" s="1">
+        <v>2554</v>
+      </c>
+      <c r="N2" s="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2554</v>
       </c>
@@ -635,7 +638,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
@@ -664,8 +667,14 @@
       <c r="L3" s="1">
         <v>144</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" s="1">
+        <v>2555</v>
+      </c>
+      <c r="N3" s="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2554</v>
       </c>
@@ -673,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
         <v>4</v>
@@ -702,8 +711,14 @@
       <c r="L4" s="1">
         <v>144</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" s="1">
+        <v>2556</v>
+      </c>
+      <c r="N4" s="1">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2554</v>
       </c>
@@ -711,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
@@ -740,8 +755,14 @@
       <c r="L5" s="1">
         <v>144</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" s="1">
+        <v>2557</v>
+      </c>
+      <c r="N5" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2554</v>
       </c>
@@ -749,7 +770,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -778,8 +799,14 @@
       <c r="L6" s="1">
         <v>144</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6" s="1">
+        <v>2560</v>
+      </c>
+      <c r="N6" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2554</v>
       </c>
@@ -787,7 +814,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
@@ -816,8 +843,14 @@
       <c r="L7" s="1">
         <v>144</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" s="1">
+        <v>2561</v>
+      </c>
+      <c r="N7" s="1">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>2555</v>
       </c>
@@ -825,7 +858,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -854,8 +887,14 @@
       <c r="L8" s="1">
         <v>272</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8" s="1">
+        <v>2562</v>
+      </c>
+      <c r="N8" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>2555</v>
       </c>
@@ -863,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
@@ -892,8 +931,14 @@
       <c r="L9" s="1">
         <v>272</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9" s="1">
+        <v>2563</v>
+      </c>
+      <c r="N9" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>2555</v>
       </c>
@@ -901,7 +946,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
         <v>5</v>
@@ -930,8 +975,14 @@
       <c r="L10" s="1">
         <v>272</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" s="1">
+        <v>2564</v>
+      </c>
+      <c r="N10" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>2555</v>
       </c>
@@ -939,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -968,8 +1019,14 @@
       <c r="L11" s="1">
         <v>272</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" s="1">
+        <v>2565</v>
+      </c>
+      <c r="N11" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>2555</v>
       </c>
@@ -977,7 +1034,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
@@ -1006,8 +1063,9 @@
       <c r="L12" s="1">
         <v>272</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>2555</v>
       </c>
@@ -1015,7 +1073,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -1044,8 +1102,9 @@
       <c r="L13" s="1">
         <v>272</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>2555</v>
       </c>
@@ -1053,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
@@ -1082,8 +1141,9 @@
       <c r="L14" s="1">
         <v>272</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>2555</v>
       </c>
@@ -1091,7 +1151,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -1121,7 +1181,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>2555</v>
       </c>
@@ -1129,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
@@ -1167,7 +1227,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -1205,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1">
         <v>2</v>
@@ -1243,7 +1303,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D19" s="1">
         <v>3</v>
@@ -1281,7 +1341,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D20" s="1">
         <v>7</v>
@@ -1319,7 +1379,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -1357,7 +1417,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
@@ -1395,7 +1455,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -1433,7 +1493,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1">
         <v>2</v>
@@ -1471,7 +1531,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -1509,7 +1569,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1">
         <v>2</v>
@@ -1547,7 +1607,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1">
         <v>1</v>
@@ -1585,7 +1645,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D28" s="1">
         <v>2</v>
@@ -1623,7 +1683,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -1661,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D30" s="1">
         <v>2</v>
@@ -1699,7 +1759,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -1737,7 +1797,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D32" s="1">
         <v>2</v>
@@ -1775,7 +1835,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D33" s="1">
         <v>7</v>
@@ -1813,7 +1873,7 @@
         <v>2</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D34" s="1">
         <v>8</v>
@@ -1851,7 +1911,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
@@ -1889,7 +1949,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
@@ -1927,7 +1987,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D37" s="1">
         <v>2</v>
@@ -1965,7 +2025,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
@@ -2003,7 +2063,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D39" s="1">
         <v>2</v>
@@ -2041,7 +2101,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
@@ -2079,7 +2139,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D41" s="1">
         <v>2</v>
@@ -2117,7 +2177,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -2155,7 +2215,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
@@ -2193,7 +2253,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D44" s="1">
         <v>2</v>
@@ -2231,7 +2291,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
@@ -2269,7 +2329,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D46" s="1">
         <v>2</v>
@@ -2307,7 +2367,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
@@ -2345,7 +2405,7 @@
         <v>2</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D48" s="1">
         <v>2</v>
@@ -2383,7 +2443,7 @@
         <v>2</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
@@ -2421,7 +2481,7 @@
         <v>2</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D50" s="1">
         <v>2</v>
@@ -2459,7 +2519,7 @@
         <v>2</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D51" s="1">
         <v>1</v>
@@ -2497,7 +2557,7 @@
         <v>2</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D52" s="1">
         <v>2</v>
@@ -2535,7 +2595,7 @@
         <v>2</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D53" s="1">
         <v>1</v>
@@ -2573,7 +2633,7 @@
         <v>2</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D54" s="1">
         <v>2</v>
@@ -2611,7 +2671,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D55" s="1">
         <v>1</v>
@@ -2649,7 +2709,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D56" s="1">
         <v>2</v>
@@ -2687,7 +2747,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D57" s="1">
         <v>1</v>
@@ -2725,7 +2785,7 @@
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D58" s="1">
         <v>2</v>
@@ -2763,7 +2823,7 @@
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D59" s="1">
         <v>1</v>
@@ -2801,7 +2861,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D60" s="1">
         <v>2</v>
@@ -2839,7 +2899,7 @@
         <v>2</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D61" s="1">
         <v>1</v>
@@ -2877,7 +2937,7 @@
         <v>2</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D62" s="1">
         <v>2</v>
@@ -2915,7 +2975,7 @@
         <v>2</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D63" s="1">
         <v>2</v>
@@ -2953,7 +3013,7 @@
         <v>2</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D64" s="1">
         <v>1</v>
@@ -2991,7 +3051,7 @@
         <v>2</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D65" s="1">
         <v>2</v>
@@ -3029,7 +3089,7 @@
         <v>2</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D66" s="1">
         <v>3</v>
@@ -3067,7 +3127,7 @@
         <v>2</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D67" s="1">
         <v>1</v>
@@ -3105,7 +3165,7 @@
         <v>2</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D68" s="1">
         <v>2</v>
@@ -3143,7 +3203,7 @@
         <v>2</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D69" s="1">
         <v>1</v>
@@ -3181,7 +3241,7 @@
         <v>2</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D70" s="1">
         <v>2</v>
@@ -3219,7 +3279,7 @@
         <v>1</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D71" s="1">
         <v>1</v>
@@ -3257,7 +3317,7 @@
         <v>1</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D72" s="1">
         <v>2</v>
@@ -3295,7 +3355,7 @@
         <v>1</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D73" s="1">
         <v>1</v>
@@ -3333,7 +3393,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D74" s="1">
         <v>2</v>
@@ -3371,7 +3431,7 @@
         <v>1</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D75" s="1">
         <v>1</v>
@@ -3409,7 +3469,7 @@
         <v>1</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D76" s="1">
         <v>1</v>
@@ -3447,7 +3507,7 @@
         <v>1</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D77" s="1">
         <v>2</v>
@@ -3485,7 +3545,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D78" s="1">
         <v>1</v>
@@ -3523,7 +3583,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D79" s="1">
         <v>2</v>
@@ -3561,7 +3621,7 @@
         <v>2</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D80" s="1">
         <v>1</v>
@@ -3599,7 +3659,7 @@
         <v>2</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D81" s="1">
         <v>2</v>
@@ -3637,7 +3697,7 @@
         <v>2</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D82" s="1">
         <v>1</v>
@@ -3675,7 +3735,7 @@
         <v>2</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D83" s="1">
         <v>2</v>
@@ -3713,7 +3773,7 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D84" s="1">
         <v>1</v>
@@ -3751,7 +3811,7 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D85" s="1">
         <v>2</v>
@@ -3789,7 +3849,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D86" s="1">
         <v>2</v>
@@ -3827,7 +3887,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D87" s="1">
         <v>1</v>
@@ -3865,7 +3925,7 @@
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D88" s="1">
         <v>1</v>
@@ -3903,7 +3963,7 @@
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D89" s="1">
         <v>2</v>
@@ -3941,7 +4001,7 @@
         <v>1</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D90" s="1">
         <v>1</v>
@@ -3979,7 +4039,7 @@
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D91" s="1">
         <v>2</v>
@@ -4017,7 +4077,7 @@
         <v>2</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D92" s="1">
         <v>1</v>
@@ -4055,7 +4115,7 @@
         <v>2</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D93" s="1">
         <v>2</v>
@@ -4093,7 +4153,7 @@
         <v>2</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D94" s="1">
         <v>1</v>
@@ -4131,7 +4191,7 @@
         <v>2</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D95" s="1">
         <v>2</v>
@@ -4169,7 +4229,7 @@
         <v>2</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D96" s="1">
         <v>3</v>
@@ -4207,7 +4267,7 @@
         <v>2</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D97" s="1">
         <v>4</v>
@@ -4245,7 +4305,7 @@
         <v>2</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D98" s="1">
         <v>1</v>
@@ -4283,7 +4343,7 @@
         <v>2</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D99" s="1">
         <v>2</v>
@@ -4321,7 +4381,7 @@
         <v>1</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D100" s="1">
         <v>1</v>
@@ -4359,7 +4419,7 @@
         <v>1</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D101" s="1">
         <v>2</v>
@@ -4397,7 +4457,7 @@
         <v>1</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D102" s="1">
         <v>1</v>
@@ -4435,7 +4495,7 @@
         <v>1</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D103" s="1">
         <v>2</v>
@@ -4473,7 +4533,7 @@
         <v>1</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D104" s="1">
         <v>1</v>
@@ -4511,7 +4571,7 @@
         <v>1</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D105" s="1">
         <v>2</v>
@@ -4549,7 +4609,7 @@
         <v>2</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D106" s="1">
         <v>1</v>
@@ -4587,7 +4647,7 @@
         <v>2</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D107" s="1">
         <v>2</v>
@@ -4625,7 +4685,7 @@
         <v>2</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D108" s="1">
         <v>1</v>
@@ -4663,7 +4723,7 @@
         <v>2</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D109" s="1">
         <v>2</v>
@@ -4701,7 +4761,7 @@
         <v>2</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D110" s="1">
         <v>1</v>
@@ -4739,7 +4799,7 @@
         <v>2</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D111" s="1">
         <v>2</v>
@@ -4777,7 +4837,7 @@
         <v>1</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D112" s="1">
         <v>1</v>
@@ -4798,7 +4858,7 @@
         <v>1372</v>
       </c>
       <c r="J112" s="1">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="K112" s="1">
         <v>7</v>
@@ -4815,7 +4875,7 @@
         <v>1</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D113" s="1">
         <v>2</v>
@@ -4836,7 +4896,7 @@
         <v>1372</v>
       </c>
       <c r="J113" s="1">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="K113" s="1">
         <v>7</v>
@@ -4853,7 +4913,7 @@
         <v>1</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D114" s="1">
         <v>21</v>
@@ -4874,7 +4934,7 @@
         <v>1372</v>
       </c>
       <c r="J114" s="1">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="K114" s="1">
         <v>7</v>
@@ -4891,7 +4951,7 @@
         <v>1</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D115" s="1">
         <v>1</v>
@@ -4912,7 +4972,7 @@
         <v>1372</v>
       </c>
       <c r="J115" s="1">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="K115" s="1">
         <v>7</v>
@@ -4929,7 +4989,7 @@
         <v>1</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D116" s="1">
         <v>2</v>
@@ -4950,7 +5010,7 @@
         <v>1372</v>
       </c>
       <c r="J116" s="1">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="K116" s="1">
         <v>7</v>
@@ -4967,7 +5027,7 @@
         <v>1</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D117" s="1">
         <v>1</v>
@@ -4988,7 +5048,7 @@
         <v>1372</v>
       </c>
       <c r="J117" s="1">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="K117" s="1">
         <v>7</v>
@@ -5005,7 +5065,7 @@
         <v>1</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D118" s="1">
         <v>2</v>
@@ -5026,7 +5086,7 @@
         <v>1372</v>
       </c>
       <c r="J118" s="1">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="K118" s="1">
         <v>7</v>
@@ -5036,536 +5096,200 @@
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A119" s="2">
-        <v>2565</v>
-      </c>
-      <c r="B119" s="2">
-        <v>2</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D119" s="1">
-        <v>1</v>
-      </c>
-      <c r="E119" s="1">
-        <v>8</v>
-      </c>
-      <c r="F119" s="1">
-        <v>0</v>
-      </c>
-      <c r="G119" s="1">
-        <v>108</v>
-      </c>
-      <c r="H119" s="1">
-        <v>1728</v>
-      </c>
-      <c r="I119" s="1">
-        <v>1372</v>
-      </c>
-      <c r="J119" s="1">
-        <v>21</v>
-      </c>
-      <c r="K119" s="1">
-        <v>14</v>
-      </c>
-      <c r="L119" s="1">
-        <v>0</v>
-      </c>
+      <c r="A119" s="2"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="1"/>
+      <c r="J119" s="1"/>
+      <c r="K119" s="1"/>
+      <c r="L119" s="1"/>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A120" s="2">
-        <v>2565</v>
-      </c>
-      <c r="B120" s="2">
-        <v>2</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D120" s="1">
-        <v>2</v>
-      </c>
-      <c r="E120" s="1">
-        <v>8</v>
-      </c>
-      <c r="F120" s="1">
-        <v>0</v>
-      </c>
-      <c r="G120" s="1">
-        <v>108</v>
-      </c>
-      <c r="H120" s="1">
-        <v>1728</v>
-      </c>
-      <c r="I120" s="1">
-        <v>1372</v>
-      </c>
-      <c r="J120" s="1">
-        <v>21</v>
-      </c>
-      <c r="K120" s="1">
-        <v>14</v>
-      </c>
-      <c r="L120" s="1">
-        <v>0</v>
-      </c>
+      <c r="A120" s="2"/>
+      <c r="B120" s="2"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="1"/>
+      <c r="E120" s="1"/>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1"/>
+      <c r="J120" s="1"/>
+      <c r="K120" s="1"/>
+      <c r="L120" s="1"/>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A121" s="2">
-        <v>2565</v>
-      </c>
-      <c r="B121" s="2">
-        <v>2</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D121" s="1">
-        <v>1</v>
-      </c>
-      <c r="E121" s="1">
-        <v>15</v>
-      </c>
-      <c r="F121" s="1">
-        <v>0</v>
-      </c>
-      <c r="G121" s="1">
-        <v>108</v>
-      </c>
-      <c r="H121" s="1">
-        <v>1728</v>
-      </c>
-      <c r="I121" s="1">
-        <v>1372</v>
-      </c>
-      <c r="J121" s="1">
-        <v>21</v>
-      </c>
-      <c r="K121" s="1">
-        <v>14</v>
-      </c>
-      <c r="L121" s="1">
-        <v>0</v>
-      </c>
+      <c r="A121" s="2"/>
+      <c r="B121" s="2"/>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="1"/>
+      <c r="J121" s="1"/>
+      <c r="K121" s="1"/>
+      <c r="L121" s="1"/>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A122" s="2">
-        <v>2565</v>
-      </c>
-      <c r="B122" s="2">
-        <v>2</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D122" s="1">
-        <v>2</v>
-      </c>
-      <c r="E122" s="1">
-        <v>2</v>
-      </c>
-      <c r="F122" s="1">
-        <v>0</v>
-      </c>
-      <c r="G122" s="1">
-        <v>108</v>
-      </c>
-      <c r="H122" s="1">
-        <v>1728</v>
-      </c>
-      <c r="I122" s="1">
-        <v>1372</v>
-      </c>
-      <c r="J122" s="1">
-        <v>21</v>
-      </c>
-      <c r="K122" s="1">
-        <v>14</v>
-      </c>
-      <c r="L122" s="1">
-        <v>0</v>
-      </c>
+      <c r="A122" s="2"/>
+      <c r="B122" s="2"/>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="1"/>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+      <c r="I122" s="1"/>
+      <c r="J122" s="1"/>
+      <c r="K122" s="1"/>
+      <c r="L122" s="1"/>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A123" s="2">
-        <v>2565</v>
-      </c>
-      <c r="B123" s="2">
-        <v>2</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D123" s="1">
-        <v>1</v>
-      </c>
-      <c r="E123" s="1">
-        <v>15</v>
-      </c>
-      <c r="F123" s="1">
-        <v>0</v>
-      </c>
-      <c r="G123" s="1">
-        <v>108</v>
-      </c>
-      <c r="H123" s="1">
-        <v>1728</v>
-      </c>
-      <c r="I123" s="1">
-        <v>1372</v>
-      </c>
-      <c r="J123" s="1">
-        <v>21</v>
-      </c>
-      <c r="K123" s="1">
-        <v>14</v>
-      </c>
-      <c r="L123" s="1">
-        <v>0</v>
-      </c>
+      <c r="A123" s="2"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="1"/>
+      <c r="D123" s="1"/>
+      <c r="E123" s="1"/>
+      <c r="F123" s="1"/>
+      <c r="G123" s="1"/>
+      <c r="H123" s="1"/>
+      <c r="I123" s="1"/>
+      <c r="J123" s="1"/>
+      <c r="K123" s="1"/>
+      <c r="L123" s="1"/>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A124" s="2">
-        <v>2565</v>
-      </c>
-      <c r="B124" s="2">
-        <v>2</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D124" s="1">
-        <v>2</v>
-      </c>
-      <c r="E124" s="1">
-        <v>2</v>
-      </c>
-      <c r="F124" s="1">
-        <v>0</v>
-      </c>
-      <c r="G124" s="1">
-        <v>108</v>
-      </c>
-      <c r="H124" s="1">
-        <v>1728</v>
-      </c>
-      <c r="I124" s="1">
-        <v>1372</v>
-      </c>
-      <c r="J124" s="1">
-        <v>21</v>
-      </c>
-      <c r="K124" s="1">
-        <v>14</v>
-      </c>
-      <c r="L124" s="1">
-        <v>0</v>
-      </c>
+      <c r="A124" s="2"/>
+      <c r="B124" s="2"/>
+      <c r="C124" s="1"/>
+      <c r="D124" s="1"/>
+      <c r="E124" s="1"/>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
+      <c r="I124" s="1"/>
+      <c r="J124" s="1"/>
+      <c r="K124" s="1"/>
+      <c r="L124" s="1"/>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A125" s="2">
-        <v>2565</v>
-      </c>
-      <c r="B125" s="2">
-        <v>2</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D125" s="1">
-        <v>1</v>
-      </c>
-      <c r="E125" s="1">
-        <v>15</v>
-      </c>
-      <c r="F125" s="1">
-        <v>0</v>
-      </c>
-      <c r="G125" s="1">
-        <v>108</v>
-      </c>
-      <c r="H125" s="1">
-        <v>1728</v>
-      </c>
-      <c r="I125" s="1">
-        <v>1372</v>
-      </c>
-      <c r="J125" s="1">
-        <v>21</v>
-      </c>
-      <c r="K125" s="1">
-        <v>14</v>
-      </c>
-      <c r="L125" s="1">
-        <v>0</v>
-      </c>
+      <c r="A125" s="2"/>
+      <c r="B125" s="2"/>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+      <c r="E125" s="1"/>
+      <c r="F125" s="1"/>
+      <c r="G125" s="1"/>
+      <c r="H125" s="1"/>
+      <c r="I125" s="1"/>
+      <c r="J125" s="1"/>
+      <c r="K125" s="1"/>
+      <c r="L125" s="1"/>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A126" s="2">
-        <v>2565</v>
-      </c>
-      <c r="B126" s="2">
-        <v>2</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D126" s="1">
-        <v>2</v>
-      </c>
-      <c r="E126" s="1">
-        <v>2</v>
-      </c>
-      <c r="F126" s="1">
-        <v>0</v>
-      </c>
-      <c r="G126" s="1">
-        <v>108</v>
-      </c>
-      <c r="H126" s="1">
-        <v>1728</v>
-      </c>
-      <c r="I126" s="1">
-        <v>1372</v>
-      </c>
-      <c r="J126" s="1">
-        <v>21</v>
-      </c>
-      <c r="K126" s="1">
-        <v>14</v>
-      </c>
-      <c r="L126" s="1">
-        <v>0</v>
-      </c>
+      <c r="A126" s="2"/>
+      <c r="B126" s="2"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+      <c r="I126" s="1"/>
+      <c r="J126" s="1"/>
+      <c r="K126" s="1"/>
+      <c r="L126" s="1"/>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A127" s="2">
-        <v>2565</v>
-      </c>
-      <c r="B127" s="2">
-        <v>2</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D127" s="1">
-        <v>1</v>
-      </c>
-      <c r="E127" s="1">
-        <v>10</v>
-      </c>
-      <c r="F127" s="1">
-        <v>0</v>
-      </c>
-      <c r="G127" s="1">
-        <v>108</v>
-      </c>
-      <c r="H127" s="1">
-        <v>1728</v>
-      </c>
-      <c r="I127" s="1">
-        <v>1372</v>
-      </c>
-      <c r="J127" s="1">
-        <v>21</v>
-      </c>
-      <c r="K127" s="1">
-        <v>14</v>
-      </c>
-      <c r="L127" s="1">
-        <v>0</v>
-      </c>
+      <c r="A127" s="2"/>
+      <c r="B127" s="2"/>
+      <c r="C127" s="1"/>
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+      <c r="F127" s="1"/>
+      <c r="G127" s="1"/>
+      <c r="H127" s="1"/>
+      <c r="I127" s="1"/>
+      <c r="J127" s="1"/>
+      <c r="K127" s="1"/>
+      <c r="L127" s="1"/>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A128" s="2">
-        <v>2565</v>
-      </c>
-      <c r="B128" s="2">
-        <v>2</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D128" s="1">
-        <v>2</v>
-      </c>
-      <c r="E128" s="1">
-        <v>10</v>
-      </c>
-      <c r="F128" s="1">
-        <v>0</v>
-      </c>
-      <c r="G128" s="1">
-        <v>108</v>
-      </c>
-      <c r="H128" s="1">
-        <v>1728</v>
-      </c>
-      <c r="I128" s="1">
-        <v>1372</v>
-      </c>
-      <c r="J128" s="1">
-        <v>21</v>
-      </c>
-      <c r="K128" s="1">
-        <v>14</v>
-      </c>
-      <c r="L128" s="1">
-        <v>0</v>
-      </c>
+      <c r="A128" s="2"/>
+      <c r="B128" s="2"/>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+      <c r="H128" s="1"/>
+      <c r="I128" s="1"/>
+      <c r="J128" s="1"/>
+      <c r="K128" s="1"/>
+      <c r="L128" s="1"/>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A129" s="2">
-        <v>2565</v>
-      </c>
-      <c r="B129" s="2">
-        <v>2</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D129" s="1">
-        <v>1</v>
-      </c>
-      <c r="E129" s="1">
-        <v>8</v>
-      </c>
-      <c r="F129" s="1">
-        <v>0</v>
-      </c>
-      <c r="G129" s="1">
-        <v>108</v>
-      </c>
-      <c r="H129" s="1">
-        <v>1728</v>
-      </c>
-      <c r="I129" s="1">
-        <v>1372</v>
-      </c>
-      <c r="J129" s="1">
-        <v>21</v>
-      </c>
-      <c r="K129" s="1">
-        <v>14</v>
-      </c>
-      <c r="L129" s="1">
-        <v>0</v>
-      </c>
+      <c r="A129" s="2"/>
+      <c r="B129" s="2"/>
+      <c r="C129" s="1"/>
+      <c r="D129" s="1"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="1"/>
+      <c r="G129" s="1"/>
+      <c r="H129" s="1"/>
+      <c r="I129" s="1"/>
+      <c r="J129" s="1"/>
+      <c r="K129" s="1"/>
+      <c r="L129" s="1"/>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A130" s="2">
-        <v>2565</v>
-      </c>
-      <c r="B130" s="2">
-        <v>2</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D130" s="1">
-        <v>2</v>
-      </c>
-      <c r="E130" s="1">
-        <v>5</v>
-      </c>
-      <c r="F130" s="1">
-        <v>0</v>
-      </c>
-      <c r="G130" s="1">
-        <v>108</v>
-      </c>
-      <c r="H130" s="1">
-        <v>1728</v>
-      </c>
-      <c r="I130" s="1">
-        <v>1372</v>
-      </c>
-      <c r="J130" s="1">
-        <v>21</v>
-      </c>
-      <c r="K130" s="1">
-        <v>14</v>
-      </c>
-      <c r="L130" s="1">
-        <v>0</v>
-      </c>
+      <c r="A130" s="2"/>
+      <c r="B130" s="2"/>
+      <c r="C130" s="1"/>
+      <c r="D130" s="1"/>
+      <c r="E130" s="1"/>
+      <c r="F130" s="1"/>
+      <c r="G130" s="1"/>
+      <c r="H130" s="1"/>
+      <c r="I130" s="1"/>
+      <c r="J130" s="1"/>
+      <c r="K130" s="1"/>
+      <c r="L130" s="1"/>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A131" s="2">
-        <v>2565</v>
-      </c>
-      <c r="B131" s="2">
-        <v>2</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D131" s="1">
-        <v>1</v>
-      </c>
-      <c r="E131" s="1">
-        <v>18</v>
-      </c>
-      <c r="F131" s="1">
-        <v>0</v>
-      </c>
-      <c r="G131" s="1">
-        <v>108</v>
-      </c>
-      <c r="H131" s="1">
-        <v>1728</v>
-      </c>
-      <c r="I131" s="1">
-        <v>1372</v>
-      </c>
-      <c r="J131" s="1">
-        <v>21</v>
-      </c>
-      <c r="K131" s="1">
-        <v>14</v>
-      </c>
-      <c r="L131" s="1">
-        <v>0</v>
-      </c>
+      <c r="A131" s="2"/>
+      <c r="B131" s="2"/>
+      <c r="C131" s="1"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
+      <c r="F131" s="1"/>
+      <c r="G131" s="1"/>
+      <c r="H131" s="1"/>
+      <c r="I131" s="1"/>
+      <c r="J131" s="1"/>
+      <c r="K131" s="1"/>
+      <c r="L131" s="1"/>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A132" s="2">
-        <v>2565</v>
-      </c>
-      <c r="B132" s="2">
-        <v>2</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D132" s="1">
-        <v>2</v>
-      </c>
-      <c r="E132" s="1">
-        <v>5</v>
-      </c>
-      <c r="F132" s="1">
-        <v>0</v>
-      </c>
-      <c r="G132" s="1">
-        <v>108</v>
-      </c>
-      <c r="H132" s="1">
-        <v>1728</v>
-      </c>
-      <c r="I132" s="1">
-        <v>1372</v>
-      </c>
-      <c r="J132" s="1">
-        <v>21</v>
-      </c>
-      <c r="K132" s="1">
-        <v>14</v>
-      </c>
-      <c r="L132" s="1">
-        <v>0</v>
-      </c>
+      <c r="A132" s="2"/>
+      <c r="B132" s="2"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="1"/>
+      <c r="J132" s="1"/>
+      <c r="K132" s="1"/>
+      <c r="L132" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>